<commit_message>
move old excel files to old folder, review latest exel file
</commit_message>
<xml_diff>
--- a/ICD-10 conversions_5_28_20.xlsx
+++ b/ICD-10 conversions_5_28_20.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elianagk/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shutfle1\Desktop\Johns-Hopkins-Overuse-Project-with-Segal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A90C1D73-83FE-FA48-AF1D-6990BD87960C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="460" windowWidth="24020" windowHeight="15000" tabRatio="856" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3900" yWindow="460" windowWidth="24020" windowHeight="15000" tabRatio="856" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="READ ME" sheetId="4" r:id="rId1"/>
@@ -46,7 +45,7 @@
     <definedName name="OLE_LINK3" localSheetId="1">'Indicator Descriptions'!$B$19</definedName>
     <definedName name="OLE_LINK4" localSheetId="1">'Indicator Descriptions'!$B$20</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2533,7 +2532,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="43">
     <font>
       <sz val="12"/>
@@ -4095,6 +4094,15 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="29" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="40" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -4130,15 +4138,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4585,24 +4584,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A33"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="98.5" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="22">
+    <row r="1" spans="1:1" ht="21">
       <c r="A1" s="16" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="34">
+    <row r="2" spans="1:1" ht="31">
       <c r="A2" s="17" t="s">
         <v>268</v>
       </c>
@@ -4628,42 +4627,42 @@
         <v>269</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="17">
+    <row r="8" spans="1:1">
       <c r="A8" s="18" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="17">
+    <row r="9" spans="1:1">
       <c r="A9" s="17" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="17">
+    <row r="10" spans="1:1">
       <c r="A10" s="17" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="17">
+    <row r="11" spans="1:1">
       <c r="A11" s="17" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="17">
+    <row r="12" spans="1:1">
       <c r="A12" s="17" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="17">
+    <row r="13" spans="1:1">
       <c r="A13" s="18" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="17">
+    <row r="14" spans="1:1">
       <c r="A14" s="17" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="17">
+    <row r="15" spans="1:1">
       <c r="A15" s="17" t="s">
         <v>179</v>
       </c>
@@ -4681,32 +4680,32 @@
     <row r="18" spans="1:1">
       <c r="A18" s="17"/>
     </row>
-    <row r="19" spans="1:1" ht="51">
+    <row r="19" spans="1:1" ht="46.5">
       <c r="A19" s="17" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="17">
+    <row r="20" spans="1:1">
       <c r="A20" s="20" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="17">
+    <row r="21" spans="1:1">
       <c r="A21" s="17" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="17">
+    <row r="22" spans="1:1">
       <c r="A22" s="17" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="17">
+    <row r="23" spans="1:1">
       <c r="A23" s="17" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="17">
+    <row r="24" spans="1:1">
       <c r="A24" s="17" t="s">
         <v>275</v>
       </c>
@@ -4721,27 +4720,27 @@
         <v>273</v>
       </c>
     </row>
-    <row r="27" spans="1:1" ht="17">
+    <row r="27" spans="1:1">
       <c r="A27" s="20" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="28" spans="1:1" ht="17">
+    <row r="28" spans="1:1">
       <c r="A28" s="17" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="29" spans="1:1" ht="17">
+    <row r="29" spans="1:1">
       <c r="A29" s="17" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="30" spans="1:1" ht="17">
+    <row r="30" spans="1:1">
       <c r="A30" s="17" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="31" spans="1:1" ht="17">
+    <row r="31" spans="1:1">
       <c r="A31" s="17" t="s">
         <v>275</v>
       </c>
@@ -4763,15 +4762,15 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK389"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="6" style="216" customWidth="1"/>
     <col min="2" max="2" width="21.6640625" style="217" customWidth="1"/>
@@ -4797,21 +4796,21 @@
   <sheetData>
     <row r="1" spans="1:37">
       <c r="T1" s="2"/>
-      <c r="U1" s="382" t="s">
+      <c r="U1" s="385" t="s">
         <v>554</v>
       </c>
-      <c r="V1" s="382"/>
-      <c r="W1" s="382"/>
-      <c r="X1" s="382"/>
-      <c r="Y1" s="382"/>
-      <c r="Z1" s="382"/>
-      <c r="AA1" s="382"/>
-      <c r="AB1" s="383" t="s">
+      <c r="V1" s="385"/>
+      <c r="W1" s="385"/>
+      <c r="X1" s="385"/>
+      <c r="Y1" s="385"/>
+      <c r="Z1" s="385"/>
+      <c r="AA1" s="385"/>
+      <c r="AB1" s="386" t="s">
         <v>555</v>
       </c>
-      <c r="AC1" s="383"/>
-      <c r="AD1" s="383"/>
-      <c r="AE1" s="383"/>
+      <c r="AC1" s="386"/>
+      <c r="AD1" s="386"/>
+      <c r="AE1" s="386"/>
       <c r="AF1" s="334"/>
       <c r="AG1" s="334"/>
       <c r="AH1" s="334"/>
@@ -4821,29 +4820,29 @@
     </row>
     <row r="2" spans="1:37">
       <c r="T2" s="335"/>
-      <c r="U2" s="384" t="s">
+      <c r="U2" s="387" t="s">
         <v>547</v>
       </c>
-      <c r="V2" s="384"/>
-      <c r="W2" s="384"/>
-      <c r="X2" s="385" t="s">
+      <c r="V2" s="387"/>
+      <c r="W2" s="387"/>
+      <c r="X2" s="388" t="s">
         <v>550</v>
       </c>
-      <c r="Y2" s="386"/>
-      <c r="Z2" s="386"/>
-      <c r="AA2" s="387"/>
-      <c r="AB2" s="388" t="s">
+      <c r="Y2" s="389"/>
+      <c r="Z2" s="389"/>
+      <c r="AA2" s="390"/>
+      <c r="AB2" s="391" t="s">
         <v>547</v>
       </c>
-      <c r="AC2" s="389"/>
-      <c r="AD2" s="389"/>
-      <c r="AE2" s="390"/>
-      <c r="AF2" s="379" t="s">
+      <c r="AC2" s="392"/>
+      <c r="AD2" s="392"/>
+      <c r="AE2" s="393"/>
+      <c r="AF2" s="382" t="s">
         <v>556</v>
       </c>
-      <c r="AG2" s="380"/>
-      <c r="AH2" s="380"/>
-      <c r="AI2" s="381"/>
+      <c r="AG2" s="383"/>
+      <c r="AH2" s="383"/>
+      <c r="AI2" s="384"/>
       <c r="AJ2" s="345"/>
       <c r="AK2" s="345"/>
     </row>
@@ -5027,7 +5026,7 @@
       <c r="AJ4" s="361" t="s">
         <v>576</v>
       </c>
-      <c r="AK4" s="391" t="s">
+      <c r="AK4" s="379" t="s">
         <v>572</v>
       </c>
     </row>
@@ -5105,7 +5104,7 @@
       <c r="AJ5" s="361" t="s">
         <v>567</v>
       </c>
-      <c r="AK5" s="392" t="s">
+      <c r="AK5" s="380" t="s">
         <v>602</v>
       </c>
     </row>
@@ -5193,7 +5192,7 @@
       <c r="AJ6" s="361" t="s">
         <v>567</v>
       </c>
-      <c r="AK6" s="393"/>
+      <c r="AK6" s="381"/>
     </row>
     <row r="7" spans="1:37" s="48" customFormat="1" ht="93.75" customHeight="1">
       <c r="A7" s="202">
@@ -5356,7 +5355,7 @@
       </c>
       <c r="AK8" s="362"/>
     </row>
-    <row r="9" spans="1:37" s="48" customFormat="1" ht="105">
+    <row r="9" spans="1:37" s="48" customFormat="1" ht="91">
       <c r="A9" s="202">
         <v>6</v>
       </c>
@@ -5516,7 +5515,7 @@
       </c>
       <c r="AK10" s="361"/>
     </row>
-    <row r="11" spans="1:37" s="48" customFormat="1" ht="90">
+    <row r="11" spans="1:37" s="48" customFormat="1" ht="78">
       <c r="A11" s="202">
         <v>8</v>
       </c>
@@ -5988,7 +5987,7 @@
       </c>
       <c r="AK16" s="361"/>
     </row>
-    <row r="17" spans="1:37" s="48" customFormat="1" ht="105">
+    <row r="17" spans="1:37" s="48" customFormat="1" ht="104">
       <c r="A17" s="202">
         <v>14</v>
       </c>
@@ -6064,7 +6063,7 @@
       </c>
       <c r="AK17" s="361"/>
     </row>
-    <row r="18" spans="1:37" s="48" customFormat="1" ht="120">
+    <row r="18" spans="1:37" s="48" customFormat="1" ht="104">
       <c r="A18" s="202">
         <v>15</v>
       </c>
@@ -6144,7 +6143,7 @@
       </c>
       <c r="AK18" s="361"/>
     </row>
-    <row r="19" spans="1:37" s="48" customFormat="1" ht="90">
+    <row r="19" spans="1:37" s="48" customFormat="1" ht="78">
       <c r="A19" s="202">
         <v>16</v>
       </c>
@@ -6222,7 +6221,7 @@
       </c>
       <c r="AK19" s="361"/>
     </row>
-    <row r="20" spans="1:37" s="48" customFormat="1" ht="180">
+    <row r="20" spans="1:37" s="48" customFormat="1" ht="156">
       <c r="A20" s="202">
         <v>17</v>
       </c>
@@ -6529,7 +6528,7 @@
       </c>
       <c r="AK23" s="345"/>
     </row>
-    <row r="24" spans="1:37" ht="221">
+    <row r="24" spans="1:37" ht="201.5">
       <c r="A24" s="202">
         <v>21</v>
       </c>
@@ -6598,7 +6597,7 @@
       </c>
       <c r="AK24" s="345"/>
     </row>
-    <row r="25" spans="1:37" ht="105">
+    <row r="25" spans="1:37" ht="91">
       <c r="A25" s="202">
         <v>22</v>
       </c>
@@ -10619,7 +10618,7 @@
       <c r="G389" s="371"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:L25">
+  <sortState ref="A4:L25">
     <sortCondition ref="I4:I25"/>
   </sortState>
   <mergeCells count="7">
@@ -10635,7 +10634,7 @@
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="K8" r:id="rId1" display="https://www.sciencedirect.com/science/article/pii/S0735109713006980?via%3Dihub" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="K8" r:id="rId1" display="https://www.sciencedirect.com/science/article/pii/S0735109713006980?via%3Dihub"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId2"/>
@@ -10644,14 +10643,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CP127"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="20.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.5" customWidth="1"/>
@@ -17569,7 +17568,7 @@
       <c r="CO71" s="3"/>
       <c r="CP71" s="3"/>
     </row>
-    <row r="72" spans="1:94" s="30" customFormat="1" ht="409.6">
+    <row r="72" spans="1:94" s="30" customFormat="1" ht="409.5">
       <c r="A72" s="327">
         <v>12</v>
       </c>
@@ -21259,12 +21258,12 @@
       <c r="AR127" s="180"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:CP1" xr:uid="{00000000-0009-0000-0000-000002000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:CP121">
+  <autoFilter ref="A1:CP1">
+    <sortState ref="A2:CP121">
       <sortCondition ref="A1:A121"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D120">
+  <sortState ref="A2:D120">
     <sortCondition ref="A2:A120"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -21273,14 +21272,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CR13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="33" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="33" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="19.33203125" customWidth="1"/>
     <col min="3" max="3" width="16" style="1" customWidth="1"/>
@@ -21290,7 +21289,7 @@
     <col min="7" max="22" width="33" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:96" s="48" customFormat="1" ht="15">
+    <row r="1" spans="1:96" s="48" customFormat="1" ht="13.5">
       <c r="A1" s="138" t="s">
         <v>0</v>
       </c>
@@ -21400,7 +21399,7 @@
       <c r="CQ1" s="44"/>
       <c r="CR1" s="44"/>
     </row>
-    <row r="2" spans="1:96" s="24" customFormat="1" ht="34">
+    <row r="2" spans="1:96" s="24" customFormat="1" ht="31">
       <c r="A2" s="143">
         <v>10</v>
       </c>
@@ -21962,14 +21961,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DQ167"/>
   <sheetViews>
     <sheetView topLeftCell="A100" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="20.25" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="20.25" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="20.83203125" style="48" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.83203125" style="48" customWidth="1"/>
@@ -36657,26 +36656,26 @@
       <c r="AP167" s="179"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C98">
+  <sortState ref="A2:C98">
     <sortCondition ref="A2:A98"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="C78" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
-    <hyperlink ref="C79" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
-    <hyperlink ref="C80" r:id="rId3" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
-    <hyperlink ref="C81" r:id="rId4" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
-    <hyperlink ref="C82" r:id="rId5" xr:uid="{00000000-0004-0000-0400-000004000000}"/>
-    <hyperlink ref="C83" r:id="rId6" xr:uid="{00000000-0004-0000-0400-000005000000}"/>
-    <hyperlink ref="C84" r:id="rId7" xr:uid="{00000000-0004-0000-0400-000006000000}"/>
-    <hyperlink ref="C85" r:id="rId8" xr:uid="{00000000-0004-0000-0400-000007000000}"/>
-    <hyperlink ref="C86" r:id="rId9" xr:uid="{00000000-0004-0000-0400-000008000000}"/>
-    <hyperlink ref="C87" r:id="rId10" xr:uid="{00000000-0004-0000-0400-000009000000}"/>
-    <hyperlink ref="C88" r:id="rId11" xr:uid="{00000000-0004-0000-0400-00000A000000}"/>
-    <hyperlink ref="C89" r:id="rId12" xr:uid="{00000000-0004-0000-0400-00000B000000}"/>
-    <hyperlink ref="C90" r:id="rId13" xr:uid="{00000000-0004-0000-0400-00000C000000}"/>
-    <hyperlink ref="C91" r:id="rId14" xr:uid="{00000000-0004-0000-0400-00000D000000}"/>
-    <hyperlink ref="C92" r:id="rId15" xr:uid="{00000000-0004-0000-0400-00000E000000}"/>
-    <hyperlink ref="C93" r:id="rId16" xr:uid="{00000000-0004-0000-0400-00000F000000}"/>
+    <hyperlink ref="C78" r:id="rId1"/>
+    <hyperlink ref="C79" r:id="rId2"/>
+    <hyperlink ref="C80" r:id="rId3"/>
+    <hyperlink ref="C81" r:id="rId4"/>
+    <hyperlink ref="C82" r:id="rId5"/>
+    <hyperlink ref="C83" r:id="rId6"/>
+    <hyperlink ref="C84" r:id="rId7"/>
+    <hyperlink ref="C85" r:id="rId8"/>
+    <hyperlink ref="C86" r:id="rId9"/>
+    <hyperlink ref="C87" r:id="rId10"/>
+    <hyperlink ref="C88" r:id="rId11"/>
+    <hyperlink ref="C89" r:id="rId12"/>
+    <hyperlink ref="C90" r:id="rId13"/>
+    <hyperlink ref="C91" r:id="rId14"/>
+    <hyperlink ref="C92" r:id="rId15"/>
+    <hyperlink ref="C93" r:id="rId16"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId17"/>
@@ -36684,15 +36683,15 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG182"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H40" sqref="H40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="20.25" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="20.25" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="23.5" style="280" customWidth="1"/>
     <col min="2" max="2" width="28.33203125" style="37" customWidth="1"/>
@@ -39883,29 +39882,29 @@
       <c r="E182" s="303"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AG1" xr:uid="{00000000-0009-0000-0000-000005000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AG61">
+  <autoFilter ref="A1:AG1">
+    <sortState ref="A2:AG61">
       <sortCondition ref="A1:A61"/>
     </sortState>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="E24" r:id="rId1" display="I50.814 Right heart failure due to left heart failure" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
-    <hyperlink ref="E45" r:id="rId2" display="R55 Syncope and collapse" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
-    <hyperlink ref="E50" r:id="rId3" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
-    <hyperlink ref="E47" r:id="rId4" xr:uid="{00000000-0004-0000-0500-000003000000}"/>
-    <hyperlink ref="E30" r:id="rId5" xr:uid="{00000000-0004-0000-0500-000004000000}"/>
-    <hyperlink ref="E31" r:id="rId6" xr:uid="{00000000-0004-0000-0500-000005000000}"/>
-    <hyperlink ref="E32" r:id="rId7" xr:uid="{00000000-0004-0000-0500-000006000000}"/>
-    <hyperlink ref="E33" r:id="rId8" xr:uid="{00000000-0004-0000-0500-000007000000}"/>
-    <hyperlink ref="E34" r:id="rId9" xr:uid="{00000000-0004-0000-0500-000008000000}"/>
-    <hyperlink ref="E35" r:id="rId10" xr:uid="{00000000-0004-0000-0500-000009000000}"/>
-    <hyperlink ref="E36" r:id="rId11" xr:uid="{00000000-0004-0000-0500-00000A000000}"/>
-    <hyperlink ref="E37" r:id="rId12" xr:uid="{00000000-0004-0000-0500-00000B000000}"/>
-    <hyperlink ref="E38" r:id="rId13" xr:uid="{00000000-0004-0000-0500-00000C000000}"/>
-    <hyperlink ref="E39" r:id="rId14" xr:uid="{00000000-0004-0000-0500-00000D000000}"/>
-    <hyperlink ref="E40" r:id="rId15" xr:uid="{00000000-0004-0000-0500-00000E000000}"/>
-    <hyperlink ref="E41" r:id="rId16" xr:uid="{00000000-0004-0000-0500-00000F000000}"/>
-    <hyperlink ref="E42" r:id="rId17" xr:uid="{00000000-0004-0000-0500-000010000000}"/>
+    <hyperlink ref="E24" r:id="rId1" display="I50.814 Right heart failure due to left heart failure"/>
+    <hyperlink ref="E45" r:id="rId2" display="R55 Syncope and collapse"/>
+    <hyperlink ref="E50" r:id="rId3"/>
+    <hyperlink ref="E47" r:id="rId4"/>
+    <hyperlink ref="E30" r:id="rId5"/>
+    <hyperlink ref="E31" r:id="rId6"/>
+    <hyperlink ref="E32" r:id="rId7"/>
+    <hyperlink ref="E33" r:id="rId8"/>
+    <hyperlink ref="E34" r:id="rId9"/>
+    <hyperlink ref="E35" r:id="rId10"/>
+    <hyperlink ref="E36" r:id="rId11"/>
+    <hyperlink ref="E37" r:id="rId12"/>
+    <hyperlink ref="E38" r:id="rId13"/>
+    <hyperlink ref="E39" r:id="rId14"/>
+    <hyperlink ref="E40" r:id="rId15"/>
+    <hyperlink ref="E41" r:id="rId16"/>
+    <hyperlink ref="E42" r:id="rId17"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId18"/>
@@ -39913,26 +39912,26 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C1AA588-8BB4-7F4C-8CB3-0D45460F0A3F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A36" sqref="A1:A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="98" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
make note on icd excel liste for 5/28 about 22 icd pcs codes
</commit_message>
<xml_diff>
--- a/ICD-10 conversions_5_28_20.xlsx
+++ b/ICD-10 conversions_5_28_20.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elianagk/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shutfle1\Desktop\Johns-Hopkins-Overuse-Project-with-Segal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A90C1D73-83FE-FA48-AF1D-6990BD87960C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="460" windowWidth="24020" windowHeight="15000" tabRatio="856" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3900" yWindow="460" windowWidth="24020" windowHeight="15000" tabRatio="856" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="READ ME" sheetId="4" r:id="rId1"/>
@@ -46,7 +45,7 @@
     <definedName name="OLE_LINK3" localSheetId="1">'Indicator Descriptions'!$B$19</definedName>
     <definedName name="OLE_LINK4" localSheetId="1">'Indicator Descriptions'!$B$20</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -64,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1340" uniqueCount="603">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1341" uniqueCount="604">
   <si>
     <t>Working Number</t>
   </si>
@@ -2529,11 +2528,14 @@
 This is how we handle time for sinusitis (7/8)
 TIME C VARIANT. The eligible population is defined by inclusionary and exclusionary codes that are time-bound but are not time-bound to the POP date. </t>
   </si>
+  <si>
+    <t>SH: there are 6 icd-10-pcs listed in the code: JS please confirm and edit how you want this table to look accordingly--right now there are 3 codes in 1 row--consider making 1 code per row per best practices</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="43">
     <font>
       <sz val="12"/>
@@ -4095,6 +4097,15 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="29" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="40" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -4130,15 +4141,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4585,24 +4587,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A33"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="98.5" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="22">
+    <row r="1" spans="1:1" ht="21">
       <c r="A1" s="16" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="34">
+    <row r="2" spans="1:1" ht="31">
       <c r="A2" s="17" t="s">
         <v>268</v>
       </c>
@@ -4628,42 +4630,42 @@
         <v>269</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="17">
+    <row r="8" spans="1:1">
       <c r="A8" s="18" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="17">
+    <row r="9" spans="1:1">
       <c r="A9" s="17" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="17">
+    <row r="10" spans="1:1">
       <c r="A10" s="17" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="17">
+    <row r="11" spans="1:1">
       <c r="A11" s="17" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="17">
+    <row r="12" spans="1:1">
       <c r="A12" s="17" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="17">
+    <row r="13" spans="1:1">
       <c r="A13" s="18" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="17">
+    <row r="14" spans="1:1">
       <c r="A14" s="17" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="17">
+    <row r="15" spans="1:1">
       <c r="A15" s="17" t="s">
         <v>179</v>
       </c>
@@ -4681,32 +4683,32 @@
     <row r="18" spans="1:1">
       <c r="A18" s="17"/>
     </row>
-    <row r="19" spans="1:1" ht="51">
+    <row r="19" spans="1:1" ht="46.5">
       <c r="A19" s="17" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="17">
+    <row r="20" spans="1:1">
       <c r="A20" s="20" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="17">
+    <row r="21" spans="1:1">
       <c r="A21" s="17" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="17">
+    <row r="22" spans="1:1">
       <c r="A22" s="17" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="17">
+    <row r="23" spans="1:1">
       <c r="A23" s="17" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="17">
+    <row r="24" spans="1:1">
       <c r="A24" s="17" t="s">
         <v>275</v>
       </c>
@@ -4721,27 +4723,27 @@
         <v>273</v>
       </c>
     </row>
-    <row r="27" spans="1:1" ht="17">
+    <row r="27" spans="1:1">
       <c r="A27" s="20" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="28" spans="1:1" ht="17">
+    <row r="28" spans="1:1">
       <c r="A28" s="17" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="29" spans="1:1" ht="17">
+    <row r="29" spans="1:1">
       <c r="A29" s="17" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="30" spans="1:1" ht="17">
+    <row r="30" spans="1:1">
       <c r="A30" s="17" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="31" spans="1:1" ht="17">
+    <row r="31" spans="1:1">
       <c r="A31" s="17" t="s">
         <v>275</v>
       </c>
@@ -4763,15 +4765,15 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK389"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
+    <sheetView topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AL25" sqref="AL25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="6" style="216" customWidth="1"/>
     <col min="2" max="2" width="21.6640625" style="217" customWidth="1"/>
@@ -4797,21 +4799,21 @@
   <sheetData>
     <row r="1" spans="1:37">
       <c r="T1" s="2"/>
-      <c r="U1" s="382" t="s">
+      <c r="U1" s="385" t="s">
         <v>554</v>
       </c>
-      <c r="V1" s="382"/>
-      <c r="W1" s="382"/>
-      <c r="X1" s="382"/>
-      <c r="Y1" s="382"/>
-      <c r="Z1" s="382"/>
-      <c r="AA1" s="382"/>
-      <c r="AB1" s="383" t="s">
+      <c r="V1" s="385"/>
+      <c r="W1" s="385"/>
+      <c r="X1" s="385"/>
+      <c r="Y1" s="385"/>
+      <c r="Z1" s="385"/>
+      <c r="AA1" s="385"/>
+      <c r="AB1" s="386" t="s">
         <v>555</v>
       </c>
-      <c r="AC1" s="383"/>
-      <c r="AD1" s="383"/>
-      <c r="AE1" s="383"/>
+      <c r="AC1" s="386"/>
+      <c r="AD1" s="386"/>
+      <c r="AE1" s="386"/>
       <c r="AF1" s="334"/>
       <c r="AG1" s="334"/>
       <c r="AH1" s="334"/>
@@ -4821,29 +4823,29 @@
     </row>
     <row r="2" spans="1:37">
       <c r="T2" s="335"/>
-      <c r="U2" s="384" t="s">
+      <c r="U2" s="387" t="s">
         <v>547</v>
       </c>
-      <c r="V2" s="384"/>
-      <c r="W2" s="384"/>
-      <c r="X2" s="385" t="s">
+      <c r="V2" s="387"/>
+      <c r="W2" s="387"/>
+      <c r="X2" s="388" t="s">
         <v>550</v>
       </c>
-      <c r="Y2" s="386"/>
-      <c r="Z2" s="386"/>
-      <c r="AA2" s="387"/>
-      <c r="AB2" s="388" t="s">
+      <c r="Y2" s="389"/>
+      <c r="Z2" s="389"/>
+      <c r="AA2" s="390"/>
+      <c r="AB2" s="391" t="s">
         <v>547</v>
       </c>
-      <c r="AC2" s="389"/>
-      <c r="AD2" s="389"/>
-      <c r="AE2" s="390"/>
-      <c r="AF2" s="379" t="s">
+      <c r="AC2" s="392"/>
+      <c r="AD2" s="392"/>
+      <c r="AE2" s="393"/>
+      <c r="AF2" s="382" t="s">
         <v>556</v>
       </c>
-      <c r="AG2" s="380"/>
-      <c r="AH2" s="380"/>
-      <c r="AI2" s="381"/>
+      <c r="AG2" s="383"/>
+      <c r="AH2" s="383"/>
+      <c r="AI2" s="384"/>
       <c r="AJ2" s="345"/>
       <c r="AK2" s="345"/>
     </row>
@@ -5027,7 +5029,7 @@
       <c r="AJ4" s="361" t="s">
         <v>576</v>
       </c>
-      <c r="AK4" s="391" t="s">
+      <c r="AK4" s="379" t="s">
         <v>572</v>
       </c>
     </row>
@@ -5105,7 +5107,7 @@
       <c r="AJ5" s="361" t="s">
         <v>567</v>
       </c>
-      <c r="AK5" s="392" t="s">
+      <c r="AK5" s="380" t="s">
         <v>602</v>
       </c>
     </row>
@@ -5193,7 +5195,7 @@
       <c r="AJ6" s="361" t="s">
         <v>567</v>
       </c>
-      <c r="AK6" s="393"/>
+      <c r="AK6" s="381"/>
     </row>
     <row r="7" spans="1:37" s="48" customFormat="1" ht="93.75" customHeight="1">
       <c r="A7" s="202">
@@ -5356,7 +5358,7 @@
       </c>
       <c r="AK8" s="362"/>
     </row>
-    <row r="9" spans="1:37" s="48" customFormat="1" ht="105">
+    <row r="9" spans="1:37" s="48" customFormat="1" ht="91">
       <c r="A9" s="202">
         <v>6</v>
       </c>
@@ -5516,7 +5518,7 @@
       </c>
       <c r="AK10" s="361"/>
     </row>
-    <row r="11" spans="1:37" s="48" customFormat="1" ht="90">
+    <row r="11" spans="1:37" s="48" customFormat="1" ht="78">
       <c r="A11" s="202">
         <v>8</v>
       </c>
@@ -5988,7 +5990,7 @@
       </c>
       <c r="AK16" s="361"/>
     </row>
-    <row r="17" spans="1:37" s="48" customFormat="1" ht="105">
+    <row r="17" spans="1:37" s="48" customFormat="1" ht="104">
       <c r="A17" s="202">
         <v>14</v>
       </c>
@@ -6064,7 +6066,7 @@
       </c>
       <c r="AK17" s="361"/>
     </row>
-    <row r="18" spans="1:37" s="48" customFormat="1" ht="120">
+    <row r="18" spans="1:37" s="48" customFormat="1" ht="104">
       <c r="A18" s="202">
         <v>15</v>
       </c>
@@ -6144,7 +6146,7 @@
       </c>
       <c r="AK18" s="361"/>
     </row>
-    <row r="19" spans="1:37" s="48" customFormat="1" ht="90">
+    <row r="19" spans="1:37" s="48" customFormat="1" ht="78">
       <c r="A19" s="202">
         <v>16</v>
       </c>
@@ -6222,7 +6224,7 @@
       </c>
       <c r="AK19" s="361"/>
     </row>
-    <row r="20" spans="1:37" s="48" customFormat="1" ht="180">
+    <row r="20" spans="1:37" s="48" customFormat="1" ht="156">
       <c r="A20" s="202">
         <v>17</v>
       </c>
@@ -6529,7 +6531,7 @@
       </c>
       <c r="AK23" s="345"/>
     </row>
-    <row r="24" spans="1:37" ht="221">
+    <row r="24" spans="1:37" ht="201.5">
       <c r="A24" s="202">
         <v>21</v>
       </c>
@@ -6598,7 +6600,7 @@
       </c>
       <c r="AK24" s="345"/>
     </row>
-    <row r="25" spans="1:37" ht="105">
+    <row r="25" spans="1:37" ht="91">
       <c r="A25" s="202">
         <v>22</v>
       </c>
@@ -10619,7 +10621,7 @@
       <c r="G389" s="371"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:L25">
+  <sortState ref="A4:L25">
     <sortCondition ref="I4:I25"/>
   </sortState>
   <mergeCells count="7">
@@ -10635,7 +10637,7 @@
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="K8" r:id="rId1" display="https://www.sciencedirect.com/science/article/pii/S0735109713006980?via%3Dihub" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="K8" r:id="rId1" display="https://www.sciencedirect.com/science/article/pii/S0735109713006980?via%3Dihub"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId2"/>
@@ -10644,14 +10646,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CP127"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView topLeftCell="A109" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C125" sqref="C125"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="20.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.5" customWidth="1"/>
@@ -17569,7 +17571,7 @@
       <c r="CO71" s="3"/>
       <c r="CP71" s="3"/>
     </row>
-    <row r="72" spans="1:94" s="30" customFormat="1" ht="409.6">
+    <row r="72" spans="1:94" s="30" customFormat="1" ht="409.5">
       <c r="A72" s="327">
         <v>12</v>
       </c>
@@ -21259,12 +21261,12 @@
       <c r="AR127" s="180"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:CP1" xr:uid="{00000000-0009-0000-0000-000002000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:CP121">
+  <autoFilter ref="A1:CP1">
+    <sortState ref="A2:CP121">
       <sortCondition ref="A1:A121"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D120">
+  <sortState ref="A2:D120">
     <sortCondition ref="A2:A120"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -21273,14 +21275,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CR13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="33" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="33" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="19.33203125" customWidth="1"/>
     <col min="3" max="3" width="16" style="1" customWidth="1"/>
@@ -21290,7 +21292,7 @@
     <col min="7" max="22" width="33" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:96" s="48" customFormat="1" ht="15">
+    <row r="1" spans="1:96" s="48" customFormat="1" ht="13.5">
       <c r="A1" s="138" t="s">
         <v>0</v>
       </c>
@@ -21400,7 +21402,7 @@
       <c r="CQ1" s="44"/>
       <c r="CR1" s="44"/>
     </row>
-    <row r="2" spans="1:96" s="24" customFormat="1" ht="34">
+    <row r="2" spans="1:96" s="24" customFormat="1" ht="31">
       <c r="A2" s="143">
         <v>10</v>
       </c>
@@ -21962,14 +21964,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DQ167"/>
   <sheetViews>
-    <sheetView topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="A140" workbookViewId="0">
+      <selection activeCell="B150" sqref="B150"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="20.25" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="20.25" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="20.83203125" style="48" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.83203125" style="48" customWidth="1"/>
@@ -34929,9 +34931,13 @@
       <c r="DQ149" s="44"/>
     </row>
     <row r="150" spans="1:121" s="56" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A150" s="48"/>
+      <c r="A150" s="48">
+        <v>22</v>
+      </c>
       <c r="B150" s="48"/>
-      <c r="C150" s="48"/>
+      <c r="C150" s="48" t="s">
+        <v>603</v>
+      </c>
       <c r="D150" s="179"/>
       <c r="E150" s="179"/>
       <c r="F150" s="179"/>
@@ -36657,26 +36663,26 @@
       <c r="AP167" s="179"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C98">
+  <sortState ref="A2:C98">
     <sortCondition ref="A2:A98"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="C78" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
-    <hyperlink ref="C79" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
-    <hyperlink ref="C80" r:id="rId3" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
-    <hyperlink ref="C81" r:id="rId4" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
-    <hyperlink ref="C82" r:id="rId5" xr:uid="{00000000-0004-0000-0400-000004000000}"/>
-    <hyperlink ref="C83" r:id="rId6" xr:uid="{00000000-0004-0000-0400-000005000000}"/>
-    <hyperlink ref="C84" r:id="rId7" xr:uid="{00000000-0004-0000-0400-000006000000}"/>
-    <hyperlink ref="C85" r:id="rId8" xr:uid="{00000000-0004-0000-0400-000007000000}"/>
-    <hyperlink ref="C86" r:id="rId9" xr:uid="{00000000-0004-0000-0400-000008000000}"/>
-    <hyperlink ref="C87" r:id="rId10" xr:uid="{00000000-0004-0000-0400-000009000000}"/>
-    <hyperlink ref="C88" r:id="rId11" xr:uid="{00000000-0004-0000-0400-00000A000000}"/>
-    <hyperlink ref="C89" r:id="rId12" xr:uid="{00000000-0004-0000-0400-00000B000000}"/>
-    <hyperlink ref="C90" r:id="rId13" xr:uid="{00000000-0004-0000-0400-00000C000000}"/>
-    <hyperlink ref="C91" r:id="rId14" xr:uid="{00000000-0004-0000-0400-00000D000000}"/>
-    <hyperlink ref="C92" r:id="rId15" xr:uid="{00000000-0004-0000-0400-00000E000000}"/>
-    <hyperlink ref="C93" r:id="rId16" xr:uid="{00000000-0004-0000-0400-00000F000000}"/>
+    <hyperlink ref="C78" r:id="rId1"/>
+    <hyperlink ref="C79" r:id="rId2"/>
+    <hyperlink ref="C80" r:id="rId3"/>
+    <hyperlink ref="C81" r:id="rId4"/>
+    <hyperlink ref="C82" r:id="rId5"/>
+    <hyperlink ref="C83" r:id="rId6"/>
+    <hyperlink ref="C84" r:id="rId7"/>
+    <hyperlink ref="C85" r:id="rId8"/>
+    <hyperlink ref="C86" r:id="rId9"/>
+    <hyperlink ref="C87" r:id="rId10"/>
+    <hyperlink ref="C88" r:id="rId11"/>
+    <hyperlink ref="C89" r:id="rId12"/>
+    <hyperlink ref="C90" r:id="rId13"/>
+    <hyperlink ref="C91" r:id="rId14"/>
+    <hyperlink ref="C92" r:id="rId15"/>
+    <hyperlink ref="C93" r:id="rId16"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId17"/>
@@ -36684,15 +36690,15 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG182"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="20.25" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="20.25" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="23.5" style="280" customWidth="1"/>
     <col min="2" max="2" width="28.33203125" style="37" customWidth="1"/>
@@ -39883,29 +39889,29 @@
       <c r="E182" s="303"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AG1" xr:uid="{00000000-0009-0000-0000-000005000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AG61">
+  <autoFilter ref="A1:AG1">
+    <sortState ref="A2:AG61">
       <sortCondition ref="A1:A61"/>
     </sortState>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="E24" r:id="rId1" display="I50.814 Right heart failure due to left heart failure" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
-    <hyperlink ref="E45" r:id="rId2" display="R55 Syncope and collapse" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
-    <hyperlink ref="E50" r:id="rId3" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
-    <hyperlink ref="E47" r:id="rId4" xr:uid="{00000000-0004-0000-0500-000003000000}"/>
-    <hyperlink ref="E30" r:id="rId5" xr:uid="{00000000-0004-0000-0500-000004000000}"/>
-    <hyperlink ref="E31" r:id="rId6" xr:uid="{00000000-0004-0000-0500-000005000000}"/>
-    <hyperlink ref="E32" r:id="rId7" xr:uid="{00000000-0004-0000-0500-000006000000}"/>
-    <hyperlink ref="E33" r:id="rId8" xr:uid="{00000000-0004-0000-0500-000007000000}"/>
-    <hyperlink ref="E34" r:id="rId9" xr:uid="{00000000-0004-0000-0500-000008000000}"/>
-    <hyperlink ref="E35" r:id="rId10" xr:uid="{00000000-0004-0000-0500-000009000000}"/>
-    <hyperlink ref="E36" r:id="rId11" xr:uid="{00000000-0004-0000-0500-00000A000000}"/>
-    <hyperlink ref="E37" r:id="rId12" xr:uid="{00000000-0004-0000-0500-00000B000000}"/>
-    <hyperlink ref="E38" r:id="rId13" xr:uid="{00000000-0004-0000-0500-00000C000000}"/>
-    <hyperlink ref="E39" r:id="rId14" xr:uid="{00000000-0004-0000-0500-00000D000000}"/>
-    <hyperlink ref="E40" r:id="rId15" xr:uid="{00000000-0004-0000-0500-00000E000000}"/>
-    <hyperlink ref="E41" r:id="rId16" xr:uid="{00000000-0004-0000-0500-00000F000000}"/>
-    <hyperlink ref="E42" r:id="rId17" xr:uid="{00000000-0004-0000-0500-000010000000}"/>
+    <hyperlink ref="E24" r:id="rId1" display="I50.814 Right heart failure due to left heart failure"/>
+    <hyperlink ref="E45" r:id="rId2" display="R55 Syncope and collapse"/>
+    <hyperlink ref="E50" r:id="rId3"/>
+    <hyperlink ref="E47" r:id="rId4"/>
+    <hyperlink ref="E30" r:id="rId5"/>
+    <hyperlink ref="E31" r:id="rId6"/>
+    <hyperlink ref="E32" r:id="rId7"/>
+    <hyperlink ref="E33" r:id="rId8"/>
+    <hyperlink ref="E34" r:id="rId9"/>
+    <hyperlink ref="E35" r:id="rId10"/>
+    <hyperlink ref="E36" r:id="rId11"/>
+    <hyperlink ref="E37" r:id="rId12"/>
+    <hyperlink ref="E38" r:id="rId13"/>
+    <hyperlink ref="E39" r:id="rId14"/>
+    <hyperlink ref="E40" r:id="rId15"/>
+    <hyperlink ref="E41" r:id="rId16"/>
+    <hyperlink ref="E42" r:id="rId17"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId18"/>
@@ -39913,26 +39919,26 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C1AA588-8BB4-7F4C-8CB3-0D45460F0A3F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A36" sqref="A1:A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="98" customWidth="1"/>
   </cols>

</xml_diff>